<commit_message>
Fix annunciator false alerts on startup
Initialize each annunciator's was_triggered state to current condition
before starting the monitor loop. This prevents announcing existing
states (like "Speed Brakes Retracted") when the monitor first loads.

Also includes expanded annunciator set (25 total).

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/CopilotAI_Annunciators.xlsx
+++ b/CopilotAI_Annunciators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnl\Documents\projects\CopilotAI\claude_shell_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC4C914B-DA93-45BE-B305-CEBD0DB7F0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B0EEB0-9F45-46F1-B05F-87DB7F24590D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57840" yWindow="-98" windowWidth="28995" windowHeight="16395" xr2:uid="{ED80179F-512A-4D75-9C06-CB1921AD6E27}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="168">
   <si>
     <t>#### FLIGHT CONTROLS</t>
   </si>
@@ -78,6 +78,468 @@
   </si>
   <si>
     <t>sw_remark:REVERSE THRUSTERS RETRACTED</t>
+  </si>
+  <si>
+    <t>#######################################################################################################</t>
+  </si>
+  <si>
+    <t>#### FLIGHT AWARENESS ALERTS ##########################################################################</t>
+  </si>
+  <si>
+    <t>#### INCLUDE ALL BELOW IN EACH CHECKLIST ##############################################################</t>
+  </si>
+  <si>
+    <t>#### NO SW_ITEM LINES OF CODE OR AIRCRAFT SPECIFIC REFERENCES #########################################</t>
+  </si>
+  <si>
+    <t>#### ALERTS TURNED ON USING - sim/cockpit/weapons/rockets_armed - DataReference #######################</t>
+  </si>
+  <si>
+    <t>#### AUTOPILOT</t>
+  </si>
+  <si>
+    <t>sw_checklist: LOCALIZER DISARMED</t>
+  </si>
+  <si>
+    <t>sw_show:sim/flightmodel2/gear/on_ground:0</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit/autopilot/mode_hnav:21:9</t>
+  </si>
+  <si>
+    <t>sw_remark:LOCALIZER DISARMED</t>
+  </si>
+  <si>
+    <t>sw_checklist: LOCALIZER ARMED</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit/autopilot/mode_hnav:9:21</t>
+  </si>
+  <si>
+    <t>sw_remark:LOCALIZER ARMED</t>
+  </si>
+  <si>
+    <t>sw_checklist: LOCALIZER CAPTURED</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit/autopilot/mode_hnav:21:22</t>
+  </si>
+  <si>
+    <t>sw_remark:LOCALIZER CAPTURED</t>
+  </si>
+  <si>
+    <t>sw_checklist: GLIDE SLOPE DISARMED</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/autopilot/glideslope_status:1:0</t>
+  </si>
+  <si>
+    <t>sw_remark:GLIDE SLOPE DISARMED</t>
+  </si>
+  <si>
+    <t>sw_checklist: ABOVE GLIDESLOPE</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/autopilot/glideslope_status:1</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/radios/indicators/nav1_vdef_dots_pilot:&gt;0.1</t>
+  </si>
+  <si>
+    <t>sw_remark:ABOVE GLIDESLOPE</t>
+  </si>
+  <si>
+    <t>sw_checklist: BELOW GLIDESLOPE</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/radios/indicators/nav1_vdef_dots_pilot:&lt;0.1</t>
+  </si>
+  <si>
+    <t>sw_remark:BELOW GLIDESLOPE</t>
+  </si>
+  <si>
+    <t>sw_checklist: GLIDE SLOPE ARMED</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/autopilot/glideslope_status:0:1</t>
+  </si>
+  <si>
+    <t>sw_remark:GLIDE SLOPE ARMED</t>
+  </si>
+  <si>
+    <t>sw_checklist: GLIDE SLOPE CAPTURED</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/autopilot/glideslope_status:1:2</t>
+  </si>
+  <si>
+    <t>sw_remark:GLIDE SLOPE CAPTURED</t>
+  </si>
+  <si>
+    <t>sw_checklist: FLIGHT LEVEL CHANGE ACTIVATED</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/autopilot/speed_status:0:2</t>
+  </si>
+  <si>
+    <t>sw_remark:FLIGHT LEVEL CHANGE ACTIVATED</t>
+  </si>
+  <si>
+    <t>sw_checklist: FLIGHT LEVEL CHANGE COMPLETED - AUTOTHROTTLE OFF</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/autopilot/speed_status:2:0</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/autopilot/autothrottle_enabled:0</t>
+  </si>
+  <si>
+    <t>sw_remark:FLIGHT LEVEL CHANGE COMPLETED - AUTOTHROTTLE OFF</t>
+  </si>
+  <si>
+    <t>sw_checklist: AUTOTHROTTLE TURNED ON</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/autopilot/autothrottle_enabled:0:1</t>
+  </si>
+  <si>
+    <t>sw_remark:AUTOTHROTTLE TURNED ON</t>
+  </si>
+  <si>
+    <t>#sw_checklist: AUTOTHROTTLE TURNED OFF</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/cockpit/weapons/rockets_armed:0</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel2/gear/on_ground:0</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/cockpit2/autopilot/autothrottle_enabled:1:0</t>
+  </si>
+  <si>
+    <t>#sw_remark:AUTOTHROTTLE TURNED OFF</t>
+  </si>
+  <si>
+    <t>#sw_checklist: PITCH MODE DISARMED</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/cockpit2/autopilot/pitch_status:1:0</t>
+  </si>
+  <si>
+    <t>#sw_remark:PITCH MODE DISARMED</t>
+  </si>
+  <si>
+    <t>#sw_checklist: PITCH MODE ARMED</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/cockpit2/autopilot/pitch_status:0:1</t>
+  </si>
+  <si>
+    <t>#sw_remark:PITCH MODE ARMED</t>
+  </si>
+  <si>
+    <t>#sw_checklist: PITCH MODE CAPTURED</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/cockpit2/autopilot/pitch_status:1:2</t>
+  </si>
+  <si>
+    <t>#sw_remark:PITCH MODE CAPTURED</t>
+  </si>
+  <si>
+    <t>#sw_checklist: ROLL MODE DISARMED</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/cockpit2/autopilot/roll_status:1:0</t>
+  </si>
+  <si>
+    <t>#sw_remark:ROLL MODE DISARMED</t>
+  </si>
+  <si>
+    <t>#sw_checklist: ROLL MODE ARMED</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/cockpit2/autopilot/roll_status:0:1</t>
+  </si>
+  <si>
+    <t>#sw_remark:ROLL MODE ARMED</t>
+  </si>
+  <si>
+    <t>#sw_checklist: ROLL MODE CAPTURED</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/cockpit2/autopilot/roll_status:1:2</t>
+  </si>
+  <si>
+    <t>#sw_remark:ROLL MODE CAPTURED</t>
+  </si>
+  <si>
+    <t>#### ALTITUDE INCREASING</t>
+  </si>
+  <si>
+    <t>sw_checklist: CHECKLIST CLIMB ABOVE 10000 FEET</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/gauges/indicators/altitude_ft_pilot:10000:10500</t>
+  </si>
+  <si>
+    <t>sw_remark:LANDING LIGHT OFF ABOVE 10000 FEET</t>
+  </si>
+  <si>
+    <t>sw_remark:SPEED AS ALLOWED BY AIR TRAFFIC CONTROL ABOVE 10000 FEET</t>
+  </si>
+  <si>
+    <t>sw_remark:CHECK CABIN ALTITUDE AND PRESSURE DIFFERENTIAL</t>
+  </si>
+  <si>
+    <t>sw_checklist: CHECKLIST CLIMB 18000 FEET AND ABOVE</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/gauges/indicators/altitude_ft_pilot:17500:18000</t>
+  </si>
+  <si>
+    <t>sw_remark:SET ALTIMETER TO 29.92 INCHES 18000 FEET AND ABOVE</t>
+  </si>
+  <si>
+    <t>#sw_checklist: CHECKLIST CLIMBING</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/y_agl:&gt;=305</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/cockpit2/gauges/indicators/vvi_fpm_pilot:&gt;1000</t>
+  </si>
+  <si>
+    <t>#sw_remark:CLIMBING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#### ALTITUDE LEVEL OFF </t>
+  </si>
+  <si>
+    <t>#sw_checklist: CHECKLIST LEVEL OFF 3000 feet AGL AND ABOVE</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/y_agl:&gt;=914</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/cockpit2/gauges/indicators/vvi_fpm_pilot:-1000|1000</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/aircraft/parts/acf_gear_deploy:0.0000</t>
+  </si>
+  <si>
+    <t>#sw_remark:LEVEL OFF</t>
+  </si>
+  <si>
+    <t>#### ALTITUDE DECREASING</t>
+  </si>
+  <si>
+    <t>#sw_checklist: CHECKLIST DESCENDING</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/cockpit2/gauges/indicators/vvi_fpm_pilot:&lt;-1000</t>
+  </si>
+  <si>
+    <t>#sw_remark:DESCENDING</t>
+  </si>
+  <si>
+    <t>sw_checklist: CHECKLIST DESCENT BELOW 18000 MSL</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/gauges/indicators/altitude_ft_pilot:18000:17500</t>
+  </si>
+  <si>
+    <t>sw_remark:SET ALTIMETER TO LOCAL SETTING BELOW 18000</t>
+  </si>
+  <si>
+    <t>sw_remark:SET CABIN ALTITUDE TO LANDING ELEVATION</t>
+  </si>
+  <si>
+    <t>sw_checklist: CHECKLIST DESCENT BELOW 10000 MSL</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/gauges/indicators/altitude_ft_pilot:10000:9500</t>
+  </si>
+  <si>
+    <t>sw_remark:DESCENDING BELOW 10,000 FEET</t>
+  </si>
+  <si>
+    <t>sw_remark:SET AIRSPEED TO 250 KNOTS OR LESS</t>
+  </si>
+  <si>
+    <t>sw_remark:TURN LANDING LIGHT ON</t>
+  </si>
+  <si>
+    <t>#sw_checklist: CHECKLIST DESCENT BELOW 8000 FEET AGL</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/y_agl:2538:2438</t>
+  </si>
+  <si>
+    <t>#sw_remark:APPROACHING GROUND 8000 FEET ABOVE</t>
+  </si>
+  <si>
+    <t>#sw_checklist: CHECKLIST DESCENT BELOW 6000 FEET AGL</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/y_agl:1929:1829</t>
+  </si>
+  <si>
+    <t>#sw_remark:APPROACHING GROUND 6000 FEET ABOVE</t>
+  </si>
+  <si>
+    <t>#sw_checklist: CHECKLIST DESCENT BELOW 4000 FEET AGL</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/y_agl:1319:1219</t>
+  </si>
+  <si>
+    <t>#sw_remark:APPROACHING GROUND 4000 FEET ABOVE</t>
+  </si>
+  <si>
+    <t>sw_checklist: CHECKLIST DESCENT BELOW 3000 FEET AGL</t>
+  </si>
+  <si>
+    <t>sw_show:sim/flightmodel/position/y_agl:1014:914</t>
+  </si>
+  <si>
+    <t>sw_remark:APPROACHING GROUND 3000 FEET ABOVE</t>
+  </si>
+  <si>
+    <t>sw_checklist: CHECKLIST DESCENT BELOW 2000 FEET AGL</t>
+  </si>
+  <si>
+    <t>sw_show:sim/flightmodel/position/y_agl:710:610</t>
+  </si>
+  <si>
+    <t>sw_remark:APPROACHING GROUND 2000 FEET ABOVE</t>
+  </si>
+  <si>
+    <t>#sw_checklist: CHECKLIST DESCENT BELOW 1000 FEET AGL</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/aircraft/parts/acf_gear_deploy:0</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/y_agl:405:305</t>
+  </si>
+  <si>
+    <t>#sw_remark:APPROACHING GROUND 1000 FEET ABOVE WITH GEAR UP</t>
+  </si>
+  <si>
+    <t>#### ALTITUDE CABIN</t>
+  </si>
+  <si>
+    <t>sw_checklist: CABIN ALTITUDE GREATER THAN 4500 FEET</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/pressurization/indicators/cabin_altitude_ft:4000:4500</t>
+  </si>
+  <si>
+    <t>sw_remark: CABIN ALTITUDE GREATER THAN 4500 FEET</t>
+  </si>
+  <si>
+    <t>sw_checklist: CABIN ALTITUDE GREATER THAN 8500 FEET</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/pressurization/indicators/cabin_altitude_ft:8000:8500</t>
+  </si>
+  <si>
+    <t>sw_remark: CABIN ALTITUDE GREATER THAN 8500 FEET</t>
+  </si>
+  <si>
+    <t>sw_checklist: CABIN ALTITUDE GREATER THAN 12500 FEET</t>
+  </si>
+  <si>
+    <t>sw_show:sim/cockpit2/pressurization/indicators/cabin_altitude_ft:12000:12500</t>
+  </si>
+  <si>
+    <t>sw_remark: WARNING - WARNING - CABIN ALTITUDE GREATER THAN 12500 FEET</t>
+  </si>
+  <si>
+    <t>#### SPEED DECREASING</t>
+  </si>
+  <si>
+    <t>#sw_checklist: LESS THAN 100 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/indicated_airspeed:120:100</t>
+  </si>
+  <si>
+    <t>#sw_remark:SPEED LESS THAN 100 KNOTS</t>
+  </si>
+  <si>
+    <t>#### SPEED INCREASING</t>
+  </si>
+  <si>
+    <t>#sw_checklist: GREATER THAN 150 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/indicated_airspeed:130:150</t>
+  </si>
+  <si>
+    <t>#sw_remark:SPEED GREATER THAN 150 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_checklist: GREATER THAN 200 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/indicated_airspeed:180:200</t>
+  </si>
+  <si>
+    <t>#sw_remark:SPEED GREATER THAN 200 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_checklist: GREATER THAN 250 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/indicated_airspeed:230:250</t>
+  </si>
+  <si>
+    <t>#sw_remark:SPEED GREATER THAN 250 KNOTS</t>
+  </si>
+  <si>
+    <t>sw_checklist: GREATER THAN 300 KNOTS</t>
+  </si>
+  <si>
+    <t>sw_show:sim/flightmodel/position/indicated_airspeed:280:300</t>
+  </si>
+  <si>
+    <t>sw_remark:SPEED GREATER THAN 300 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_checklist: GREATER THAN 350 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/indicated_airspeed:330:350</t>
+  </si>
+  <si>
+    <t>#sw_remark:SPEED GREATER THAN 350 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_checklist: GREATER THAN 400 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/indicated_airspeed:380:400</t>
+  </si>
+  <si>
+    <t>#sw_remark:SPEED GREATER THAN 400 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_checklist: GREATER THAN 450 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/indicated_airspeed:430:450</t>
+  </si>
+  <si>
+    <t>#sw_checklist: GREATER THAN 500 KNOTS</t>
+  </si>
+  <si>
+    <t>#sw_show:sim/flightmodel/position/indicated_airspeed:480:500</t>
+  </si>
+  <si>
+    <t>#sw_remark:SPEED GREATER THAN 500 KNOTS</t>
   </si>
 </sst>
 </file>
@@ -449,97 +911,1297 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06714295-7657-4541-8D94-F73187752F2E}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A21"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>5</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A114" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A116" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A120" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A122" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A124" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A125" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A126" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A127" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A129" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A130" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A131" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A132" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A134" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A135" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A136" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A137" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A139" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A140" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A141" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A142" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A144" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A146" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A148" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A149" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A150" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A151" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A152" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A154" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A155" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A156" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A157" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A158" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A159" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A161" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A162" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A163" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A164" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A165" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A166" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A168" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A170" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A171" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A172" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A173" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A174" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A175" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A176" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A178" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A180" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A181" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A182" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A183" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A184" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A185" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A187" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A188" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A189" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A190" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A191" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A192" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A194" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A195" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A196" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A197" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A198" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A199" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A200" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A202" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A203" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A204" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A205" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A206" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A208" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A209" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A210" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A211" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A212" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A214" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A215" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A216" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A217" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A218" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A220" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A221" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A222" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A223" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A224" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A226" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A227" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A228" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A229" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A230" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A232" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A233" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A234" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A235" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A236" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A237" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A239" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A241" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A242" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A243" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A244" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A246" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A247" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A248" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A249" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A251" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A252" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A253" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A254" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A256" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A258" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A259" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A260" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A261" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A262" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A264" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A266" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A267" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A268" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A269" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A270" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A272" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A273" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A274" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A275" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A276" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A278" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A279" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A280" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A281" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A282" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A284" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A285" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A286" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A287" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A288" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A290" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A291" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A292" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A293" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A294" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A296" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A297" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A298" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A299" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A300" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A302" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A303" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A304" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A305" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A306" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A308" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A309" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A310" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A311" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A312" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>